<commit_message>
[modify] post comment api
</commit_message>
<xml_diff>
--- a/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Upd003_コメント投稿.xlsx
+++ b/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Upd003_コメント投稿.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13880" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="27320" windowHeight="15360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="2" r:id="rId1"/>
@@ -51,10 +51,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
   <si>
     <t>Confidential</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>【変更履歴】</t>
@@ -64,14 +64,14 @@
     <rPh sb="3" eb="5">
       <t>リレキ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>版</t>
     <rPh sb="0" eb="1">
       <t>ハン</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>変更内容</t>
@@ -81,7 +81,7 @@
     <rPh sb="2" eb="4">
       <t>ナイヨウ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>改訂日</t>
@@ -91,7 +91,7 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>改訂者</t>
@@ -101,7 +101,7 @@
     <rPh sb="2" eb="3">
       <t>シャ</t>
     </rPh>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>設計書名</t>
@@ -111,21 +111,21 @@
     <rPh sb="3" eb="4">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>作成日</t>
     <rPh sb="0" eb="3">
       <t>サクセイビ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>作成者</t>
     <rPh sb="0" eb="3">
       <t>サクセイシャ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>改訂日</t>
@@ -135,7 +135,7 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>改訂者</t>
@@ -145,43 +145,43 @@
     <rPh sb="2" eb="3">
       <t>シャ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ID</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>備考</t>
     <rPh sb="0" eb="2">
       <t>ビコウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>必須</t>
     <rPh sb="0" eb="2">
       <t>ヒッス</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>0.0.1</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>柴</t>
     <rPh sb="0" eb="1">
       <t>シバ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ 概要</t>
     <rPh sb="2" eb="4">
       <t>ガイヨウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■使用画面</t>
@@ -191,18 +191,18 @@
     <rPh sb="3" eb="5">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>#</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>画面ID</t>
     <rPh sb="0" eb="2">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>画面名</t>
@@ -212,27 +212,27 @@
     <rPh sb="2" eb="3">
       <t>メイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ リクエスト</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ エンドポイント</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>#</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>エンドポイント</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>HTTPメソッド</t>
-    <phoneticPr fontId="7"/>
+    <phoneticPr fontId="8"/>
   </si>
   <si>
     <t>項目名(英名)</t>
@@ -245,7 +245,7 @@
     <rPh sb="4" eb="6">
       <t>エイメイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>項目名(和名)</t>
@@ -258,45 +258,45 @@
     <rPh sb="4" eb="6">
       <t>ワメイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Java型</t>
     <rPh sb="4" eb="5">
       <t>ガタ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>BigDecimal</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>List&lt;?&gt;</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>JSON型</t>
     <rPh sb="4" eb="5">
       <t>ガタ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>LocalDate</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Number</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>■ レスポンス</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>初版作成</t>
@@ -309,30 +309,30 @@
     <rPh sb="2" eb="4">
       <t>サクセイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
     <t>・body</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Boolean</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Array</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・body</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・クエリパラメータ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・以下の画面でAPIを使用する</t>
@@ -345,18 +345,18 @@
     <rPh sb="11" eb="13">
       <t>シヨウスル</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Ref_002</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>POST</t>
   </si>
   <si>
     <t>HI-04-01</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>トークテーマ詳細画面</t>
@@ -366,26 +366,26 @@
     <rPh sb="8" eb="10">
       <t>ガメン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>なし</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>isSuccess</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>成功フラグ</t>
     <rPh sb="0" eb="2">
       <t>セイコウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Boolean</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>・トークテーマの投稿を行う</t>
@@ -395,7 +395,7 @@
     <rPh sb="11" eb="12">
       <t>オコナ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
@@ -407,51 +407,102 @@
         <color theme="1"/>
         <rFont val="メイリオ"/>
         <family val="2"/>
-        <charset val="128"/>
+        <charset val="129"/>
       </rPr>
       <t>comment</t>
     </r>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Ref_003</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>中村</t>
     <rPh sb="0" eb="2">
       <t>ナカムラ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>message</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>メッセージ</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>String</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>N</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>コメント</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>userName</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ユーザ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>BigDecimal</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>talkThemeId</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>トークテーマID</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>コメント</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>0.0.2</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>リクエストから登録日時を削除。コメントの内容をレスポンスに追加。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <r>
       <t>トークテーマの評価が成功したか</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="メイリオ"/>
-        <charset val="128"/>
-      </rPr>
-      <t>（成功したら他のユーザのコメントも追加されているかもしれないので一覧取得を再度実行する？）</t>
     </r>
     <r>
       <rPr>
@@ -465,74 +516,7 @@
 True:成功(HTTPステータス:200)
 False:失敗(HTTPステータス:400)</t>
     </r>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>comment</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>コメント</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>userName</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ユーザ</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>createDatetime</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>登録日時</t>
-    <rPh sb="0" eb="4">
-      <t>トウロクニチジ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>LocalDateTime</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>BigDecimal</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>comment</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>talkThemeId</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>トークテーマID</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>コメント</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -552,6 +536,13 @@
       <name val="Yu Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="12"/>
@@ -665,12 +656,6 @@
       <sz val="11"/>
       <name val="メイリオ"/>
       <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="メイリオ"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -865,340 +850,357 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="31">
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
@@ -1206,6 +1208,13 @@
     <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="2"/>
@@ -1216,6 +1225,13 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1255,7 +1271,7 @@
         <xdr:cNvPr id="3" name="グループ化 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1274,7 +1290,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1339,7 +1355,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1404,7 +1420,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1469,7 +1485,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1534,7 +1550,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1599,7 +1615,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1664,7 +1680,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1736,7 +1752,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1808,7 +1824,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1880,7 +1896,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1952,7 +1968,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2024,7 +2040,7 @@
           <xdr:cNvPr id="15" name="正方形/長方形 14">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2117,7 +2133,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2136,7 +2152,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2201,7 +2217,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2266,7 +2282,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2331,7 +2347,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2396,7 +2412,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2461,7 +2477,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2526,7 +2542,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2598,7 +2614,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2670,7 +2686,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2742,7 +2758,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2814,7 +2830,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2886,7 +2902,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2979,7 +2995,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2998,7 +3014,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3063,7 +3079,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3128,7 +3144,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3193,7 +3209,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3258,7 +3274,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3323,7 +3339,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3388,7 +3404,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3460,7 +3476,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3532,7 +3548,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3604,7 +3620,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3676,7 +3692,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3748,7 +3764,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -4159,30 +4175,30 @@
       </c>
     </row>
     <row r="13" spans="1:26">
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="75"/>
+      <c r="V13" s="75"/>
+      <c r="W13" s="75"/>
+      <c r="X13" s="75"/>
+      <c r="Y13" s="75"/>
+      <c r="Z13" s="75"/>
     </row>
     <row r="21" spans="2:51" ht="3" customHeight="1">
       <c r="B21" s="4"/>
@@ -4242,33 +4258,33 @@
       </c>
     </row>
     <row r="27" spans="2:51">
-      <c r="AO27" s="48">
+      <c r="AO27" s="72">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(改訂日),COLUMN(改訂日),4,1),1)&amp;COUNTA(改訂日)+4)</f>
-        <v>43472</v>
-      </c>
-      <c r="AP27" s="49"/>
-      <c r="AQ27" s="49"/>
-      <c r="AR27" s="49"/>
-      <c r="AS27" s="49"/>
-      <c r="AT27" s="49"/>
-      <c r="AU27" s="49"/>
-      <c r="AV27" s="49"/>
-      <c r="AW27" s="49"/>
-      <c r="AX27" s="49"/>
-      <c r="AY27" s="49"/>
+        <v>43479</v>
+      </c>
+      <c r="AP27" s="73"/>
+      <c r="AQ27" s="73"/>
+      <c r="AR27" s="73"/>
+      <c r="AS27" s="73"/>
+      <c r="AT27" s="73"/>
+      <c r="AU27" s="73"/>
+      <c r="AV27" s="73"/>
+      <c r="AW27" s="73"/>
+      <c r="AX27" s="73"/>
+      <c r="AY27" s="73"/>
     </row>
     <row r="28" spans="2:51">
-      <c r="AR28" s="50" t="str">
+      <c r="AR28" s="74" t="str">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(版),COLUMN(版),4,1),1)&amp;COUNTA(版)+4)</f>
-        <v>0.0.1</v>
-      </c>
-      <c r="AS28" s="50"/>
-      <c r="AT28" s="50"/>
-      <c r="AU28" s="50"/>
-      <c r="AV28" s="50"/>
-      <c r="AW28" s="50"/>
-      <c r="AX28" s="50"/>
-      <c r="AY28" s="50"/>
+        <v>0.0.2</v>
+      </c>
+      <c r="AS28" s="74"/>
+      <c r="AT28" s="74"/>
+      <c r="AU28" s="74"/>
+      <c r="AV28" s="74"/>
+      <c r="AW28" s="74"/>
+      <c r="AX28" s="74"/>
+      <c r="AY28" s="74"/>
     </row>
     <row r="31" spans="2:51">
       <c r="AR31" s="6"/>
@@ -4280,7 +4296,7 @@
     <mergeCell ref="AR28:AY28"/>
     <mergeCell ref="C13:Z13"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" orientation="landscape"/>
   <extLst>
@@ -4298,7 +4314,9 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
@@ -4312,7 +4330,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="64"/>
+      <c r="A1" s="49"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4361,10 +4379,18 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="106">
+        <v>43479</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" s="25"/>
@@ -4481,7 +4507,7 @@
       <c r="E25" s="28"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="94" orientation="landscape"/>
   <extLst>
@@ -4606,14 +4632,14 @@
       <c r="AH11" s="19"/>
     </row>
     <row r="12" spans="2:81" ht="19">
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="63" t="s">
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="48" t="s">
         <v>53</v>
       </c>
       <c r="I12" s="13"/>
@@ -4737,7 +4763,7 @@
   <mergeCells count="1">
     <mergeCell ref="C12:G12"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
       <formula1>"GET,POST,PUT,DELETE"</formula1>
@@ -4759,11 +4785,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CC17"/>
+  <dimension ref="A1:CC16"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15:AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="3.125" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -4776,7 +4802,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="6.75" customHeight="1">
-      <c r="A1" s="105"/>
+      <c r="A1" s="71"/>
     </row>
     <row r="2" spans="1:81">
       <c r="BX2" s="31" t="s">
@@ -4903,56 +4929,56 @@
       </c>
     </row>
     <row r="9" spans="1:81">
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="98"/>
-      <c r="Q9" s="98"/>
-      <c r="R9" s="99"/>
-      <c r="S9" s="97"/>
-      <c r="T9" s="98"/>
-      <c r="U9" s="98"/>
-      <c r="V9" s="98"/>
-      <c r="W9" s="98"/>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="99"/>
-      <c r="Z9" s="97"/>
-      <c r="AA9" s="98"/>
-      <c r="AB9" s="98"/>
-      <c r="AC9" s="98"/>
-      <c r="AD9" s="98"/>
-      <c r="AE9" s="98"/>
-      <c r="AF9" s="99"/>
-      <c r="AG9" s="103"/>
-      <c r="AH9" s="104"/>
-      <c r="AI9" s="100"/>
-      <c r="AJ9" s="101"/>
-      <c r="AK9" s="101"/>
-      <c r="AL9" s="101"/>
-      <c r="AM9" s="101"/>
-      <c r="AN9" s="101"/>
-      <c r="AO9" s="101"/>
-      <c r="AP9" s="101"/>
-      <c r="AQ9" s="101"/>
-      <c r="AR9" s="101"/>
-      <c r="AS9" s="101"/>
-      <c r="AT9" s="101"/>
-      <c r="AU9" s="101"/>
-      <c r="AV9" s="101"/>
-      <c r="AW9" s="101"/>
-      <c r="AX9" s="102"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
+      <c r="AD9" s="80"/>
+      <c r="AE9" s="80"/>
+      <c r="AF9" s="81"/>
+      <c r="AG9" s="85"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="82"/>
+      <c r="AJ9" s="83"/>
+      <c r="AK9" s="83"/>
+      <c r="AL9" s="83"/>
+      <c r="AM9" s="83"/>
+      <c r="AN9" s="83"/>
+      <c r="AO9" s="83"/>
+      <c r="AP9" s="83"/>
+      <c r="AQ9" s="83"/>
+      <c r="AR9" s="83"/>
+      <c r="AS9" s="83"/>
+      <c r="AT9" s="83"/>
+      <c r="AU9" s="83"/>
+      <c r="AV9" s="83"/>
+      <c r="AW9" s="83"/>
+      <c r="AX9" s="84"/>
       <c r="BX9" s="30" t="s">
         <v>30</v>
       </c>
@@ -4980,11 +5006,11 @@
       </c>
     </row>
     <row r="12" spans="1:81" s="9" customFormat="1">
-      <c r="C12" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="83"/>
+      <c r="C12" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="64"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="24" t="s">
         <v>26</v>
       </c>
@@ -5043,73 +5069,73 @@
       <c r="AW12" s="24"/>
       <c r="AX12" s="19"/>
       <c r="BW12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ12" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:81" s="9" customFormat="1">
+      <c r="C13" s="66">
+        <v>1</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="BZ12" s="9" t="s">
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="88"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="96" t="s">
+        <v>30</v>
+      </c>
+      <c r="U13" s="96"/>
+      <c r="V13" s="96"/>
+      <c r="W13" s="96"/>
+      <c r="X13" s="96"/>
+      <c r="Y13" s="96"/>
+      <c r="Z13" s="96"/>
+      <c r="AA13" s="96" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:81" s="9" customFormat="1">
-      <c r="C13" s="84">
-        <v>1</v>
-      </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="60" t="s">
-        <v>75</v>
-      </c>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="61"/>
-      <c r="T13" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="U13" s="87"/>
-      <c r="V13" s="87"/>
-      <c r="W13" s="87"/>
-      <c r="X13" s="87"/>
-      <c r="Y13" s="87"/>
-      <c r="Z13" s="87"/>
-      <c r="AA13" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB13" s="87"/>
-      <c r="AC13" s="87"/>
-      <c r="AD13" s="87"/>
-      <c r="AE13" s="87"/>
-      <c r="AF13" s="87"/>
-      <c r="AG13" s="87"/>
-      <c r="AH13" s="76" t="s">
+      <c r="AB13" s="96"/>
+      <c r="AC13" s="96"/>
+      <c r="AD13" s="96"/>
+      <c r="AE13" s="96"/>
+      <c r="AF13" s="96"/>
+      <c r="AG13" s="96"/>
+      <c r="AH13" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="AI13" s="88"/>
-      <c r="AJ13" s="88"/>
-      <c r="AK13" s="88"/>
-      <c r="AL13" s="88"/>
-      <c r="AM13" s="88"/>
-      <c r="AN13" s="88"/>
-      <c r="AO13" s="88"/>
-      <c r="AP13" s="88"/>
-      <c r="AQ13" s="88"/>
-      <c r="AR13" s="88"/>
-      <c r="AS13" s="88"/>
-      <c r="AT13" s="88"/>
-      <c r="AU13" s="88"/>
-      <c r="AV13" s="88"/>
-      <c r="AW13" s="88"/>
-      <c r="AX13" s="88"/>
+      <c r="AI13" s="97"/>
+      <c r="AJ13" s="97"/>
+      <c r="AK13" s="97"/>
+      <c r="AL13" s="97"/>
+      <c r="AM13" s="97"/>
+      <c r="AN13" s="97"/>
+      <c r="AO13" s="97"/>
+      <c r="AP13" s="97"/>
+      <c r="AQ13" s="97"/>
+      <c r="AR13" s="97"/>
+      <c r="AS13" s="97"/>
+      <c r="AT13" s="97"/>
+      <c r="AU13" s="97"/>
+      <c r="AV13" s="97"/>
+      <c r="AW13" s="97"/>
+      <c r="AX13" s="97"/>
       <c r="BW13" s="9" t="s">
         <v>30</v>
       </c>
@@ -5118,66 +5144,66 @@
       </c>
     </row>
     <row r="14" spans="1:81" s="9" customFormat="1">
-      <c r="C14" s="89"/>
-      <c r="D14" s="90">
+      <c r="C14" s="69"/>
+      <c r="D14" s="70">
         <v>2</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="67" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="91" t="s">
+      <c r="E14" s="68"/>
+      <c r="F14" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="88"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="U14" s="92"/>
-      <c r="V14" s="92"/>
-      <c r="W14" s="92"/>
-      <c r="X14" s="92"/>
-      <c r="Y14" s="92"/>
-      <c r="Z14" s="93"/>
-      <c r="AA14" s="91" t="s">
+      <c r="U14" s="91"/>
+      <c r="V14" s="91"/>
+      <c r="W14" s="91"/>
+      <c r="X14" s="91"/>
+      <c r="Y14" s="91"/>
+      <c r="Z14" s="92"/>
+      <c r="AA14" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="AB14" s="92"/>
-      <c r="AC14" s="92"/>
-      <c r="AD14" s="92"/>
-      <c r="AE14" s="92"/>
-      <c r="AF14" s="92"/>
-      <c r="AG14" s="93"/>
-      <c r="AH14" s="76" t="s">
+      <c r="AB14" s="91"/>
+      <c r="AC14" s="91"/>
+      <c r="AD14" s="91"/>
+      <c r="AE14" s="91"/>
+      <c r="AF14" s="91"/>
+      <c r="AG14" s="92"/>
+      <c r="AH14" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="AI14" s="94"/>
-      <c r="AJ14" s="95"/>
-      <c r="AK14" s="95"/>
-      <c r="AL14" s="95"/>
-      <c r="AM14" s="95"/>
-      <c r="AN14" s="95"/>
-      <c r="AO14" s="95"/>
-      <c r="AP14" s="95"/>
-      <c r="AQ14" s="95"/>
-      <c r="AR14" s="95"/>
-      <c r="AS14" s="95"/>
-      <c r="AT14" s="95"/>
-      <c r="AU14" s="95"/>
-      <c r="AV14" s="95"/>
-      <c r="AW14" s="95"/>
-      <c r="AX14" s="96"/>
+      <c r="AI14" s="93"/>
+      <c r="AJ14" s="94"/>
+      <c r="AK14" s="94"/>
+      <c r="AL14" s="94"/>
+      <c r="AM14" s="94"/>
+      <c r="AN14" s="94"/>
+      <c r="AO14" s="94"/>
+      <c r="AP14" s="94"/>
+      <c r="AQ14" s="94"/>
+      <c r="AR14" s="94"/>
+      <c r="AS14" s="94"/>
+      <c r="AT14" s="94"/>
+      <c r="AU14" s="94"/>
+      <c r="AV14" s="94"/>
+      <c r="AW14" s="94"/>
+      <c r="AX14" s="95"/>
       <c r="BW14" s="9" t="s">
         <v>39</v>
       </c>
@@ -5186,13 +5212,13 @@
       </c>
     </row>
     <row r="15" spans="1:81" s="9" customFormat="1">
-      <c r="C15" s="70"/>
-      <c r="D15" s="71">
+      <c r="C15" s="52"/>
+      <c r="D15" s="53">
         <v>4</v>
       </c>
-      <c r="E15" s="72"/>
+      <c r="E15" s="54"/>
       <c r="F15" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
@@ -5200,8 +5226,8 @@
       <c r="J15" s="36"/>
       <c r="K15" s="36"/>
       <c r="L15" s="37"/>
-      <c r="M15" s="68" t="s">
-        <v>62</v>
+      <c r="M15" s="50" t="s">
+        <v>61</v>
       </c>
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
@@ -5209,43 +5235,43 @@
       <c r="Q15" s="36"/>
       <c r="R15" s="36"/>
       <c r="S15" s="37"/>
-      <c r="T15" s="73" t="s">
+      <c r="T15" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="U15" s="74"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="74"/>
-      <c r="X15" s="74"/>
-      <c r="Y15" s="74"/>
-      <c r="Z15" s="75"/>
-      <c r="AA15" s="73" t="s">
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="56"/>
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AB15" s="74"/>
-      <c r="AC15" s="74"/>
-      <c r="AD15" s="74"/>
-      <c r="AE15" s="74"/>
-      <c r="AF15" s="74"/>
-      <c r="AG15" s="75"/>
-      <c r="AH15" s="76" t="s">
+      <c r="AB15" s="56"/>
+      <c r="AC15" s="56"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="56"/>
+      <c r="AF15" s="56"/>
+      <c r="AG15" s="57"/>
+      <c r="AH15" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="AI15" s="77"/>
-      <c r="AJ15" s="78"/>
-      <c r="AK15" s="78"/>
-      <c r="AL15" s="78"/>
-      <c r="AM15" s="78"/>
-      <c r="AN15" s="78"/>
-      <c r="AO15" s="78"/>
-      <c r="AP15" s="78"/>
-      <c r="AQ15" s="78"/>
-      <c r="AR15" s="78"/>
-      <c r="AS15" s="78"/>
-      <c r="AT15" s="78"/>
-      <c r="AU15" s="78"/>
-      <c r="AV15" s="78"/>
-      <c r="AW15" s="78"/>
-      <c r="AX15" s="79"/>
+      <c r="AI15" s="59"/>
+      <c r="AJ15" s="60"/>
+      <c r="AK15" s="60"/>
+      <c r="AL15" s="60"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="60"/>
+      <c r="AO15" s="60"/>
+      <c r="AP15" s="60"/>
+      <c r="AQ15" s="60"/>
+      <c r="AR15" s="60"/>
+      <c r="AS15" s="60"/>
+      <c r="AT15" s="60"/>
+      <c r="AU15" s="60"/>
+      <c r="AV15" s="60"/>
+      <c r="AW15" s="60"/>
+      <c r="AX15" s="61"/>
       <c r="BW15" s="9" t="s">
         <v>40</v>
       </c>
@@ -5254,13 +5280,13 @@
       </c>
     </row>
     <row r="16" spans="1:81" s="9" customFormat="1">
-      <c r="C16" s="70"/>
-      <c r="D16" s="71">
+      <c r="C16" s="62"/>
+      <c r="D16" s="53">
         <v>5</v>
       </c>
-      <c r="E16" s="72"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
@@ -5268,8 +5294,8 @@
       <c r="J16" s="36"/>
       <c r="K16" s="36"/>
       <c r="L16" s="37"/>
-      <c r="M16" s="68" t="s">
-        <v>64</v>
+      <c r="M16" s="50" t="s">
+        <v>63</v>
       </c>
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
@@ -5277,114 +5303,59 @@
       <c r="Q16" s="36"/>
       <c r="R16" s="36"/>
       <c r="S16" s="37"/>
-      <c r="T16" s="73" t="s">
+      <c r="T16" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74"/>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
-      <c r="Z16" s="75"/>
-      <c r="AA16" s="73" t="s">
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AB16" s="74"/>
-      <c r="AC16" s="74"/>
-      <c r="AD16" s="74"/>
-      <c r="AE16" s="74"/>
-      <c r="AF16" s="74"/>
-      <c r="AG16" s="75"/>
-      <c r="AH16" s="76" t="s">
+      <c r="AB16" s="56"/>
+      <c r="AC16" s="56"/>
+      <c r="AD16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="AI16" s="77"/>
-      <c r="AJ16" s="78"/>
-      <c r="AK16" s="78"/>
-      <c r="AL16" s="78"/>
-      <c r="AM16" s="78"/>
-      <c r="AN16" s="78"/>
-      <c r="AO16" s="78"/>
-      <c r="AP16" s="78"/>
-      <c r="AQ16" s="78"/>
-      <c r="AR16" s="78"/>
-      <c r="AS16" s="78"/>
-      <c r="AT16" s="78"/>
-      <c r="AU16" s="78"/>
-      <c r="AV16" s="78"/>
-      <c r="AW16" s="78"/>
-      <c r="AX16" s="79"/>
+      <c r="AI16" s="59"/>
+      <c r="AJ16" s="60"/>
+      <c r="AK16" s="60"/>
+      <c r="AL16" s="60"/>
+      <c r="AM16" s="60"/>
+      <c r="AN16" s="60"/>
+      <c r="AO16" s="60"/>
+      <c r="AP16" s="60"/>
+      <c r="AQ16" s="60"/>
+      <c r="AR16" s="60"/>
+      <c r="AS16" s="60"/>
+      <c r="AT16" s="60"/>
+      <c r="AU16" s="60"/>
+      <c r="AV16" s="60"/>
+      <c r="AW16" s="60"/>
+      <c r="AX16" s="61"/>
       <c r="BZ16" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="3:78" s="9" customFormat="1">
-      <c r="C17" s="80"/>
-      <c r="D17" s="71">
-        <v>6</v>
-      </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="U17" s="74"/>
-      <c r="V17" s="74"/>
-      <c r="W17" s="74"/>
-      <c r="X17" s="74"/>
-      <c r="Y17" s="74"/>
-      <c r="Z17" s="75"/>
-      <c r="AA17" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB17" s="74"/>
-      <c r="AC17" s="74"/>
-      <c r="AD17" s="74"/>
-      <c r="AE17" s="74"/>
-      <c r="AF17" s="74"/>
-      <c r="AG17" s="75"/>
-      <c r="AH17" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI17" s="77"/>
-      <c r="AJ17" s="78"/>
-      <c r="AK17" s="78"/>
-      <c r="AL17" s="78"/>
-      <c r="AM17" s="78"/>
-      <c r="AN17" s="78"/>
-      <c r="AO17" s="78"/>
-      <c r="AP17" s="78"/>
-      <c r="AQ17" s="78"/>
-      <c r="AR17" s="78"/>
-      <c r="AS17" s="78"/>
-      <c r="AT17" s="78"/>
-      <c r="AU17" s="78"/>
-      <c r="AV17" s="78"/>
-      <c r="AW17" s="78"/>
-      <c r="AX17" s="79"/>
-      <c r="BZ17" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F13:L13"/>
+    <mergeCell ref="M13:S13"/>
+    <mergeCell ref="T13:Z13"/>
+    <mergeCell ref="AA13:AG13"/>
+    <mergeCell ref="AI13:AX13"/>
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="M14:S14"/>
+    <mergeCell ref="T14:Z14"/>
+    <mergeCell ref="AA14:AG14"/>
+    <mergeCell ref="AI14:AX14"/>
     <mergeCell ref="E9:K9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="AI9:AX9"/>
@@ -5392,20 +5363,10 @@
     <mergeCell ref="Z9:AF9"/>
     <mergeCell ref="S9:Y9"/>
     <mergeCell ref="L9:R9"/>
-    <mergeCell ref="F14:L14"/>
-    <mergeCell ref="M14:S14"/>
-    <mergeCell ref="T14:Z14"/>
-    <mergeCell ref="AA14:AG14"/>
-    <mergeCell ref="AI14:AX14"/>
-    <mergeCell ref="F13:L13"/>
-    <mergeCell ref="M13:S13"/>
-    <mergeCell ref="T13:Z13"/>
-    <mergeCell ref="AA13:AG13"/>
-    <mergeCell ref="AI13:AX13"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG9:AH9 AH13:AH17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG9:AH9 AH13:AH16">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5571,65 +5532,65 @@
         <v>1</v>
       </c>
       <c r="D9" s="47"/>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="60" t="s">
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="62" t="s">
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="62"/>
-      <c r="Z9" s="62" t="s">
+      <c r="T9" s="105"/>
+      <c r="U9" s="105"/>
+      <c r="V9" s="105"/>
+      <c r="W9" s="105"/>
+      <c r="X9" s="105"/>
+      <c r="Y9" s="105"/>
+      <c r="Z9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="62"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="62"/>
-      <c r="AE9" s="62"/>
-      <c r="AF9" s="62"/>
-      <c r="AG9" s="56" t="s">
+      <c r="AA9" s="105"/>
+      <c r="AB9" s="105"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="AH9" s="56"/>
-      <c r="AI9" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ9" s="55"/>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="55"/>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
-      <c r="AQ9" s="55"/>
-      <c r="AR9" s="55"/>
-      <c r="AS9" s="55"/>
-      <c r="AT9" s="55"/>
-      <c r="AU9" s="55"/>
-      <c r="AV9" s="55"/>
-      <c r="AW9" s="55"/>
-      <c r="AX9" s="55"/>
-      <c r="BA9" s="69"/>
+      <c r="AH9" s="103"/>
+      <c r="AI9" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ9" s="104"/>
+      <c r="AK9" s="104"/>
+      <c r="AL9" s="104"/>
+      <c r="AM9" s="104"/>
+      <c r="AN9" s="104"/>
+      <c r="AO9" s="104"/>
+      <c r="AP9" s="104"/>
+      <c r="AQ9" s="104"/>
+      <c r="AR9" s="104"/>
+      <c r="AS9" s="104"/>
+      <c r="AT9" s="104"/>
+      <c r="AU9" s="104"/>
+      <c r="AV9" s="104"/>
+      <c r="AW9" s="104"/>
+      <c r="AX9" s="104"/>
+      <c r="BA9" s="51"/>
       <c r="BX9" s="38" t="s">
         <v>30</v>
       </c>
@@ -5642,62 +5603,62 @@
         <v>2</v>
       </c>
       <c r="D10" s="47"/>
-      <c r="E10" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="61"/>
-      <c r="S10" s="67" t="s">
+      <c r="E10" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="67" t="s">
+      <c r="T10" s="88"/>
+      <c r="U10" s="88"/>
+      <c r="V10" s="88"/>
+      <c r="W10" s="88"/>
+      <c r="X10" s="88"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="61"/>
-      <c r="AG10" s="65" t="s">
+      <c r="AA10" s="88"/>
+      <c r="AB10" s="88"/>
+      <c r="AC10" s="88"/>
+      <c r="AD10" s="88"/>
+      <c r="AE10" s="88"/>
+      <c r="AF10" s="89"/>
+      <c r="AG10" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="AH10" s="66"/>
-      <c r="AI10" s="57"/>
-      <c r="AJ10" s="58"/>
-      <c r="AK10" s="58"/>
-      <c r="AL10" s="58"/>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="58"/>
-      <c r="AO10" s="58"/>
-      <c r="AP10" s="58"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="58"/>
-      <c r="AS10" s="58"/>
-      <c r="AT10" s="58"/>
-      <c r="AU10" s="58"/>
-      <c r="AV10" s="58"/>
-      <c r="AW10" s="58"/>
-      <c r="AX10" s="59"/>
+      <c r="AH10" s="102"/>
+      <c r="AI10" s="98"/>
+      <c r="AJ10" s="99"/>
+      <c r="AK10" s="99"/>
+      <c r="AL10" s="99"/>
+      <c r="AM10" s="99"/>
+      <c r="AN10" s="99"/>
+      <c r="AO10" s="99"/>
+      <c r="AP10" s="99"/>
+      <c r="AQ10" s="99"/>
+      <c r="AR10" s="99"/>
+      <c r="AS10" s="99"/>
+      <c r="AT10" s="99"/>
+      <c r="AU10" s="99"/>
+      <c r="AV10" s="99"/>
+      <c r="AW10" s="99"/>
+      <c r="AX10" s="100"/>
       <c r="BX10" s="38" t="s">
         <v>39</v>
       </c>
@@ -5705,25 +5666,99 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="2:81">
+      <c r="C11" s="46">
+        <v>3</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" s="88"/>
+      <c r="U11" s="88"/>
+      <c r="V11" s="88"/>
+      <c r="W11" s="88"/>
+      <c r="X11" s="88"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA11" s="88"/>
+      <c r="AB11" s="88"/>
+      <c r="AC11" s="88"/>
+      <c r="AD11" s="88"/>
+      <c r="AE11" s="88"/>
+      <c r="AF11" s="89"/>
+      <c r="AG11" s="101" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH11" s="102"/>
+      <c r="AI11" s="98"/>
+      <c r="AJ11" s="99"/>
+      <c r="AK11" s="99"/>
+      <c r="AL11" s="99"/>
+      <c r="AM11" s="99"/>
+      <c r="AN11" s="99"/>
+      <c r="AO11" s="99"/>
+      <c r="AP11" s="99"/>
+      <c r="AQ11" s="99"/>
+      <c r="AR11" s="99"/>
+      <c r="AS11" s="99"/>
+      <c r="AT11" s="99"/>
+      <c r="AU11" s="99"/>
+      <c r="AV11" s="99"/>
+      <c r="AW11" s="99"/>
+      <c r="AX11" s="100"/>
+      <c r="BX11" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="CA11" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="40" ht="19" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="AI11:AX11"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="L11:R11"/>
+    <mergeCell ref="S11:Y11"/>
+    <mergeCell ref="Z11:AF11"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="L9:R9"/>
+    <mergeCell ref="S9:Y9"/>
+    <mergeCell ref="Z9:AF9"/>
+    <mergeCell ref="L10:R10"/>
+    <mergeCell ref="E10:K10"/>
     <mergeCell ref="AI10:AX10"/>
     <mergeCell ref="AG10:AH10"/>
     <mergeCell ref="Z10:AF10"/>
     <mergeCell ref="S10:Y10"/>
     <mergeCell ref="AG9:AH9"/>
     <mergeCell ref="AI9:AX9"/>
-    <mergeCell ref="E9:K9"/>
-    <mergeCell ref="L9:R9"/>
-    <mergeCell ref="S9:Y9"/>
-    <mergeCell ref="Z9:AF9"/>
-    <mergeCell ref="L10:R10"/>
-    <mergeCell ref="E10:K10"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG9:AH10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG9:AH11">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>